<commit_message>
Combined ImportCourseEquiv and ImportConfig classes to form Configuration class. Made other small modifications as well.
</commit_message>
<xml_diff>
--- a/course_equivalency_list.xlsx
+++ b/course_equivalency_list.xlsx
@@ -394,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,57 +405,51 @@
     <col min="2" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="F3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>